<commit_message>
No.: proj_3_1_balancecar_wheeltec Author: xxy Description:引脚分配更新
</commit_message>
<xml_diff>
--- a/proj_3_balancecar/proj_3_1_balancecar_wheeltec/DOC/轮趣平衡小车STM32F103C8T6主控引脚资源分配.xlsx
+++ b/proj_3_balancecar/proj_3_1_balancecar_wheeltec/DOC/轮趣平衡小车STM32F103C8T6主控引脚资源分配.xlsx
@@ -4,30 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>序号</t>
   </si>
@@ -47,22 +34,25 @@
     <t>PB15/PB14/PB13/PB12</t>
   </si>
   <si>
+    <t>TB6612-AIN2/AIN1/BIN1/BIN2</t>
+  </si>
+  <si>
+    <t>普通IO</t>
+  </si>
+  <si>
+    <t>PA8/PA11</t>
+  </si>
+  <si>
+    <t>TB6612-PWMA/PWMB</t>
+  </si>
+  <si>
     <t>TB6612-PWM</t>
   </si>
   <si>
-    <t>PA8/PA11</t>
-  </si>
-  <si>
-    <t>普通IO</t>
-  </si>
-  <si>
-    <t>TB6612-普通IO</t>
-  </si>
-  <si>
     <t>PA0/PA1</t>
   </si>
   <si>
-    <t>TIM2-CH1/CH2</t>
+    <t>M1-A/B-TIM2-CH1/CH2</t>
   </si>
   <si>
     <t>电机编码器1</t>
@@ -71,7 +61,7 @@
     <t>PB6/PB7</t>
   </si>
   <si>
-    <t>TIM4-CH1/CH2</t>
+    <t>M2-A/B-TIM4-CH1/CH2</t>
   </si>
   <si>
     <t>电机编码器2</t>
@@ -80,31 +70,34 @@
     <t>PB0/PB1</t>
   </si>
   <si>
+    <t>ECHO/TRIG</t>
+  </si>
+  <si>
     <t>超声波</t>
   </si>
   <si>
     <t>PB8/PB9/PA12</t>
   </si>
   <si>
-    <t>I2C/中断引脚</t>
+    <t>I2C-SCL/SDA/INT</t>
   </si>
   <si>
     <t>MPU6050</t>
   </si>
   <si>
-    <t>OLED-I2C可复用PB8/9/蜂鸣器复用PA12,OLED支持两种</t>
+    <t>OLED-I2C可复用PB8/9/KEY2复用PA12,OLED支持两种</t>
   </si>
   <si>
     <t>PB10/PB11</t>
   </si>
   <si>
-    <t>USART3</t>
-  </si>
-  <si>
-    <t>蓝牙</t>
-  </si>
-  <si>
-    <t>预留跟K210通信</t>
+    <t>USART3-TX3/RX3</t>
+  </si>
+  <si>
+    <t>串口3-蓝牙</t>
+  </si>
+  <si>
+    <t>串口3与ESP32串口2通信</t>
   </si>
   <si>
     <t>PA4</t>
@@ -131,19 +124,29 @@
     <t>PB3/PB4/PB5/PA15</t>
   </si>
   <si>
+    <t>G/V/SCL/SDA/RES/DC
+PB3-SCK/4-MISO/5-MOSI/PA15-NSS</t>
+  </si>
+  <si>
     <t>OLED-SPI</t>
   </si>
   <si>
-    <t>五路巡迹可复用</t>
+    <t>三路巡迹复用PB3/4/5</t>
+  </si>
+  <si>
+    <t>待实物确认</t>
   </si>
   <si>
     <t>PA9/PA10</t>
   </si>
   <si>
-    <t>USART1</t>
-  </si>
-  <si>
-    <t>MicroUSB串口控制</t>
+    <t>USART1-TX1/RX1</t>
+  </si>
+  <si>
+    <t>串口1-USB串口控制</t>
+  </si>
+  <si>
+    <t>串口1与K210通信</t>
   </si>
   <si>
     <t>A13/A14</t>
@@ -155,28 +158,43 @@
     <t>不用引出</t>
   </si>
   <si>
-    <t>PA3/PA2/PA7</t>
-  </si>
-  <si>
-    <t>AO/CLK/SI</t>
-  </si>
-  <si>
-    <t>TSL1401线性CCD</t>
-  </si>
-  <si>
-    <t>G-V-AO-CLK-SI</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>预留KEY2</t>
+    <t>PA3/PA2/PA7?PB0?</t>
+  </si>
+  <si>
+    <t>USART2-AO/CLK/SI</t>
+  </si>
+  <si>
+    <t>TSL1401线性CCD/串口2</t>
+  </si>
+  <si>
+    <t>PA15复用SPI</t>
+  </si>
+  <si>
+    <t>舵机</t>
+  </si>
+  <si>
+    <t>PA7复用TSL1401</t>
+  </si>
+  <si>
+    <t>蜂鸣器</t>
+  </si>
+  <si>
+    <t>PA2/PA3复用TSL1401</t>
+  </si>
+  <si>
+    <t>USART2-TX/RX</t>
+  </si>
+  <si>
+    <t>调试串口2</t>
+  </si>
+  <si>
+    <t>串口2与OpenMV通信</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -336,7 +354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,7 +363,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,7 +713,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -707,16 +737,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -725,89 +755,89 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -821,6 +851,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1353,7 +1398,7 @@
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1388,8 +1433,11 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1398,13 +1446,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1412,14 +1460,14 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -1427,14 +1475,14 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -1443,11 +1491,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1456,16 +1506,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1473,28 +1523,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1502,12 +1552,12 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -1516,107 +1566,127 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" ht="40.5" spans="1:6">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>36</v>
+      <c r="B13" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>39</v>
+      <c r="B14" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
+      <c r="B15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="2"/>
+      <c r="B16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="8"/>
       <c r="D16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
+        <v>51</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="E17" s="2"/>
+      <c r="F17" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2"/>

</xml_diff>